<commit_message>
adjusting some more comments, making one README
</commit_message>
<xml_diff>
--- a/analysis/source/joint_spend_search_model/inf_horizon_het_results_onset_newjob_exit_rate.xlsx
+++ b/analysis/source/joint_spend_search_model/inf_horizon_het_results_onset_newjob_exit_rate.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>newjob_exit_rate_FPUC</t>
+  </si>
+  <si>
+    <t>newjob_exit_rate_no_FPUC</t>
+  </si>
   <si>
     <t>newjob_exit_rate_FPUC</t>
   </si>
@@ -40,7 +46,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -49,13 +55,15 @@
       <diagonal/>
     </border>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -74,10 +82,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">

</xml_diff>